<commit_message>
complete up to predicted graph
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stsabca-my.sharepoint.com/personal/chene_sts_ab_ca/Documents/physics/Y2/Labs/Investigation of the moments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{63221E9B-6DF3-447E-B53B-F0B8A007A6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F917895-2262-4B56-B9FC-24DB0D2BEA70}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{63221E9B-6DF3-447E-B53B-F0B8A007A6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{490A373E-204F-4522-AC0E-A0BB5E040F7F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="9060" yWindow="0" windowWidth="11070" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Predicted Graph" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Controlled variables:</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>Position of weights along ruler /m (\pm 0.001m)</t>
+  </si>
+  <si>
+    <t>PREDICTED force measured by spring scale</t>
   </si>
 </sst>
 </file>
@@ -240,6 +244,1428 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PREDICTED force measured by spring scale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="7.0000000000000007E-2"/>
+            <c:backward val="0.1"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10758062479964532"/>
+                  <c:y val="4.2801672141602437E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$3:$N$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1249999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.625</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.8749999999999991</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.625</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.7499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.8749999999999991</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.9999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.125</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.2499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.375</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.4999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.625</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.875</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.1250000000000009</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.3750000000000009</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.6249999999999991</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.7499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.875</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.1249999999999991</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.3750000000000009</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.625</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.8750000000000009</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.125</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.375</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8.625</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8.875</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.125</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9.625</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.7499999999999982</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9.875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E2C8-4387-B927-3B05191E270C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1278295936"/>
+        <c:axId val="1481420336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1278295936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.9"/>
+          <c:min val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> between weights and pivot point along ruler /m</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1481420336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1481420336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Force measured by spring</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> balance /N</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1278295936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C972303E-BC49-4138-9202-7CB5C9F6842E}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8665882" cy="6287745"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435BEC99-3BF0-C9B0-F414-6DB2D5B5806F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="L30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,9 +1949,11 @@
     <col min="11" max="11" width="22.7265625" customWidth="1"/>
     <col min="12" max="12" width="21.6328125" customWidth="1"/>
     <col min="13" max="13" width="25.1796875" customWidth="1"/>
+    <col min="14" max="14" width="29.26953125" customWidth="1"/>
+    <col min="18" max="18" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +1961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -555,8 +1983,11 @@
       <c r="M2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>10</v>
       </c>
@@ -579,8 +2010,12 @@
       <c r="M3" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3" s="11">
+        <f>0.75+(10*(L3-0.1)/0.8)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E4" s="9">
         <v>9.6999999999999993</v>
       </c>
@@ -594,8 +2029,12 @@
       <c r="M4" s="11">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4" s="11">
+        <f t="shared" ref="N4:N66" si="1">0.75+(10*(L4-0.1)/0.8)</f>
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E5" s="9">
         <v>9.4</v>
       </c>
@@ -609,8 +2048,12 @@
       <c r="M5" s="11">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N5" s="11">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E6" s="10">
         <v>9.1999999999999993</v>
       </c>
@@ -624,8 +2067,12 @@
       <c r="M6" s="11">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6" s="11">
+        <f t="shared" si="1"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K7" s="11">
         <v>24</v>
       </c>
@@ -636,8 +2083,12 @@
       <c r="M7" s="11">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7" s="11">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K8" s="11">
         <v>25</v>
       </c>
@@ -648,8 +2099,12 @@
       <c r="M8" s="11">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8" s="11">
+        <f t="shared" si="1"/>
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K9" s="11">
         <v>26</v>
       </c>
@@ -660,8 +2115,12 @@
       <c r="M9" s="11">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9" s="11">
+        <f t="shared" si="1"/>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K10" s="11">
         <v>27</v>
       </c>
@@ -672,8 +2131,12 @@
       <c r="M10" s="11">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N10" s="11">
+        <f t="shared" si="1"/>
+        <v>2.875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K11" s="11">
         <v>28</v>
       </c>
@@ -684,8 +2147,12 @@
       <c r="M11" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11" s="11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K12" s="11">
         <v>29</v>
       </c>
@@ -696,8 +2163,12 @@
       <c r="M12" s="11">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N12" s="11">
+        <f t="shared" si="1"/>
+        <v>3.1249999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K13" s="11">
         <v>30</v>
       </c>
@@ -708,8 +2179,12 @@
       <c r="M13" s="11">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N13" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2499999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K14" s="11">
         <v>31</v>
       </c>
@@ -720,8 +2195,12 @@
       <c r="M14" s="11">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N14" s="11">
+        <f t="shared" si="1"/>
+        <v>3.375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K15" s="11">
         <v>32</v>
       </c>
@@ -732,8 +2211,12 @@
       <c r="M15" s="11">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N15" s="11">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K16" s="11">
         <v>33</v>
       </c>
@@ -744,8 +2227,12 @@
       <c r="M16" s="11">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="17" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N16" s="11">
+        <f t="shared" si="1"/>
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="17" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K17" s="11">
         <v>34</v>
       </c>
@@ -756,8 +2243,12 @@
       <c r="M17" s="11">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="18" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>3.7500000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K18" s="11">
         <v>35</v>
       </c>
@@ -768,8 +2259,12 @@
       <c r="M18" s="11">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="19" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N18" s="11">
+        <f t="shared" si="1"/>
+        <v>3.8749999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K19" s="11">
         <v>36</v>
       </c>
@@ -780,8 +2275,12 @@
       <c r="M19" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N19" s="11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K20" s="11">
         <v>37</v>
       </c>
@@ -792,8 +2291,12 @@
       <c r="M20" s="11">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="21" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N20" s="11">
+        <f t="shared" si="1"/>
+        <v>4.125</v>
+      </c>
+    </row>
+    <row r="21" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K21" s="11">
         <v>38</v>
       </c>
@@ -804,8 +2307,12 @@
       <c r="M21" s="11">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="22" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N21" s="11">
+        <f t="shared" si="1"/>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="22" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K22" s="11">
         <v>39</v>
       </c>
@@ -816,8 +2323,12 @@
       <c r="M22" s="11">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="23" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N22" s="11">
+        <f t="shared" si="1"/>
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="23" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K23" s="11">
         <v>40</v>
       </c>
@@ -828,8 +2339,12 @@
       <c r="M23" s="11">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="24" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N23" s="11">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="24" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K24" s="11">
         <v>41</v>
       </c>
@@ -840,8 +2355,12 @@
       <c r="M24" s="11">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="25" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N24" s="11">
+        <f t="shared" si="1"/>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="25" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K25" s="11">
         <v>42</v>
       </c>
@@ -852,8 +2371,12 @@
       <c r="M25" s="11">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="26" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N25" s="11">
+        <f t="shared" si="1"/>
+        <v>4.7499999999999991</v>
+      </c>
+    </row>
+    <row r="26" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K26" s="11">
         <v>43</v>
       </c>
@@ -864,8 +2387,12 @@
       <c r="M26" s="11">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N26" s="11">
+        <f t="shared" si="1"/>
+        <v>4.8749999999999991</v>
+      </c>
+    </row>
+    <row r="27" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K27" s="11">
         <v>44</v>
       </c>
@@ -876,8 +2403,12 @@
       <c r="M27" s="11">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N27" s="11">
+        <f t="shared" si="1"/>
+        <v>4.9999999999999991</v>
+      </c>
+    </row>
+    <row r="28" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K28" s="11">
         <v>45</v>
       </c>
@@ -888,8 +2419,12 @@
       <c r="M28" s="11">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="29" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N28" s="11">
+        <f t="shared" si="1"/>
+        <v>5.125</v>
+      </c>
+    </row>
+    <row r="29" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K29" s="11">
         <v>46</v>
       </c>
@@ -900,8 +2435,12 @@
       <c r="M29" s="11">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="30" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N29" s="11">
+        <f t="shared" si="1"/>
+        <v>5.2499999999999991</v>
+      </c>
+    </row>
+    <row r="30" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K30" s="11">
         <v>47</v>
       </c>
@@ -912,8 +2451,12 @@
       <c r="M30" s="11">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="31" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N30" s="11">
+        <f t="shared" si="1"/>
+        <v>5.375</v>
+      </c>
+    </row>
+    <row r="31" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K31" s="11">
         <v>48</v>
       </c>
@@ -924,8 +2467,12 @@
       <c r="M31" s="11">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="32" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N31" s="11">
+        <f t="shared" si="1"/>
+        <v>5.4999999999999991</v>
+      </c>
+    </row>
+    <row r="32" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K32" s="11">
         <v>49</v>
       </c>
@@ -936,8 +2483,12 @@
       <c r="M32" s="11">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="33" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N32" s="11">
+        <f t="shared" si="1"/>
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="33" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K33" s="11">
         <v>50</v>
       </c>
@@ -948,8 +2499,12 @@
       <c r="M33" s="11">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="34" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N33" s="11">
+        <f t="shared" si="1"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="34" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K34" s="11">
         <v>51</v>
       </c>
@@ -960,8 +2515,12 @@
       <c r="M34" s="11">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="35" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N34" s="11">
+        <f t="shared" si="1"/>
+        <v>5.875</v>
+      </c>
+    </row>
+    <row r="35" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K35" s="11">
         <v>52</v>
       </c>
@@ -972,8 +2531,12 @@
       <c r="M35" s="11">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N35" s="11">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K36" s="11">
         <v>53</v>
       </c>
@@ -984,8 +2547,12 @@
       <c r="M36" s="11">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="37" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N36" s="11">
+        <f t="shared" si="1"/>
+        <v>6.1250000000000009</v>
+      </c>
+    </row>
+    <row r="37" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K37" s="11">
         <v>54</v>
       </c>
@@ -996,8 +2563,12 @@
       <c r="M37" s="11">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="38" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N37" s="11">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="38" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K38" s="11">
         <v>55</v>
       </c>
@@ -1008,8 +2579,12 @@
       <c r="M38" s="11">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="39" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N38" s="11">
+        <f t="shared" si="1"/>
+        <v>6.3750000000000009</v>
+      </c>
+    </row>
+    <row r="39" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K39" s="11">
         <v>56</v>
       </c>
@@ -1020,8 +2595,12 @@
       <c r="M39" s="11">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="40" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N39" s="11">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="40" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K40" s="11">
         <v>57</v>
       </c>
@@ -1032,8 +2611,12 @@
       <c r="M40" s="11">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="41" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N40" s="11">
+        <f t="shared" si="1"/>
+        <v>6.6249999999999991</v>
+      </c>
+    </row>
+    <row r="41" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K41" s="11">
         <v>58</v>
       </c>
@@ -1044,8 +2627,12 @@
       <c r="M41" s="11">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="42" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N41" s="11">
+        <f t="shared" si="1"/>
+        <v>6.7499999999999991</v>
+      </c>
+    </row>
+    <row r="42" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K42" s="11">
         <v>59</v>
       </c>
@@ -1056,8 +2643,12 @@
       <c r="M42" s="11">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="43" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N42" s="11">
+        <f t="shared" si="1"/>
+        <v>6.875</v>
+      </c>
+    </row>
+    <row r="43" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K43" s="11">
         <v>60</v>
       </c>
@@ -1068,8 +2659,12 @@
       <c r="M43" s="11">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="44" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N43" s="11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K44" s="11">
         <v>61</v>
       </c>
@@ -1080,8 +2675,12 @@
       <c r="M44" s="11">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="45" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N44" s="11">
+        <f t="shared" si="1"/>
+        <v>7.1249999999999991</v>
+      </c>
+    </row>
+    <row r="45" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K45" s="11">
         <v>62</v>
       </c>
@@ -1092,8 +2691,12 @@
       <c r="M45" s="11">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="46" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N45" s="11">
+        <f t="shared" si="1"/>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="46" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K46" s="11">
         <v>63</v>
       </c>
@@ -1104,8 +2707,12 @@
       <c r="M46" s="11">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="47" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N46" s="11">
+        <f t="shared" si="1"/>
+        <v>7.3750000000000009</v>
+      </c>
+    </row>
+    <row r="47" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K47" s="11">
         <v>64</v>
       </c>
@@ -1116,8 +2723,12 @@
       <c r="M47" s="11">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="48" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N47" s="11">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="48" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K48" s="11">
         <v>65</v>
       </c>
@@ -1128,8 +2739,12 @@
       <c r="M48" s="11">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="49" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N48" s="11">
+        <f t="shared" si="1"/>
+        <v>7.625</v>
+      </c>
+    </row>
+    <row r="49" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K49" s="11">
         <v>66</v>
       </c>
@@ -1140,8 +2755,12 @@
       <c r="M49" s="11">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="50" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N49" s="11">
+        <f t="shared" si="1"/>
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="50" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K50" s="11">
         <v>67</v>
       </c>
@@ -1152,8 +2771,12 @@
       <c r="M50" s="11">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="51" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N50" s="11">
+        <f t="shared" si="1"/>
+        <v>7.8750000000000009</v>
+      </c>
+    </row>
+    <row r="51" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K51" s="11">
         <v>68</v>
       </c>
@@ -1164,8 +2787,12 @@
       <c r="M51" s="11">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N51" s="11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K52" s="11">
         <v>69</v>
       </c>
@@ -1176,8 +2803,12 @@
       <c r="M52" s="11">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="53" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N52" s="11">
+        <f t="shared" si="1"/>
+        <v>8.125</v>
+      </c>
+    </row>
+    <row r="53" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K53" s="11">
         <v>70</v>
       </c>
@@ -1188,8 +2819,12 @@
       <c r="M53" s="11">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="54" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N53" s="11">
+        <f t="shared" si="1"/>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="54" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K54" s="11">
         <v>71</v>
       </c>
@@ -1200,8 +2835,12 @@
       <c r="M54" s="11">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="55" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N54" s="11">
+        <f t="shared" si="1"/>
+        <v>8.375</v>
+      </c>
+    </row>
+    <row r="55" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K55" s="11">
         <v>72</v>
       </c>
@@ -1212,8 +2851,12 @@
       <c r="M55" s="11">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="56" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N55" s="11">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="56" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K56" s="11">
         <v>73</v>
       </c>
@@ -1224,8 +2867,12 @@
       <c r="M56" s="11">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="57" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N56" s="11">
+        <f t="shared" si="1"/>
+        <v>8.625</v>
+      </c>
+    </row>
+    <row r="57" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K57" s="11">
         <v>74</v>
       </c>
@@ -1236,8 +2883,12 @@
       <c r="M57" s="11">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="58" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N57" s="11">
+        <f t="shared" si="1"/>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="58" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K58" s="11">
         <v>75</v>
       </c>
@@ -1248,8 +2899,12 @@
       <c r="M58" s="11">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="59" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N58" s="11">
+        <f t="shared" si="1"/>
+        <v>8.875</v>
+      </c>
+    </row>
+    <row r="59" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K59" s="11">
         <v>76</v>
       </c>
@@ -1260,8 +2915,12 @@
       <c r="M59" s="11">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="60" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N59" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K60" s="11">
         <v>77</v>
       </c>
@@ -1272,8 +2931,12 @@
       <c r="M60" s="11">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="61" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N60" s="11">
+        <f t="shared" si="1"/>
+        <v>9.125</v>
+      </c>
+    </row>
+    <row r="61" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K61" s="11">
         <v>78</v>
       </c>
@@ -1284,8 +2947,12 @@
       <c r="M61" s="11">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="62" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N61" s="11">
+        <f t="shared" si="1"/>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="62" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K62" s="11">
         <v>79</v>
       </c>
@@ -1296,8 +2963,12 @@
       <c r="M62" s="11">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="63" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N62" s="11">
+        <f t="shared" si="1"/>
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="63" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K63" s="11">
         <v>80</v>
       </c>
@@ -1308,8 +2979,12 @@
       <c r="M63" s="11">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="64" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N63" s="11">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="64" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K64" s="11">
         <v>81</v>
       </c>
@@ -1320,8 +2995,12 @@
       <c r="M64" s="11">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="65" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N64" s="11">
+        <f t="shared" si="1"/>
+        <v>9.625</v>
+      </c>
+    </row>
+    <row r="65" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K65" s="11">
         <v>82</v>
       </c>
@@ -1332,8 +3011,12 @@
       <c r="M65" s="11">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="66" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="N65" s="11">
+        <f t="shared" si="1"/>
+        <v>9.7499999999999982</v>
+      </c>
+    </row>
+    <row r="66" spans="11:14" x14ac:dyDescent="0.35">
       <c r="K66" s="11">
         <v>83</v>
       </c>
@@ -1343,6 +3026,10 @@
       </c>
       <c r="M66" s="11">
         <v>10</v>
+      </c>
+      <c r="N66" s="11">
+        <f t="shared" si="1"/>
+        <v>9.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete up to slope based off of exp data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stsabca-my.sharepoint.com/personal/chene_sts_ab_ca/Documents/physics/Y2/Labs/Investigation of the moments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{63221E9B-6DF3-447E-B53B-F0B8A007A6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{490A373E-204F-4522-AC0E-A0BB5E040F7F}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{63221E9B-6DF3-447E-B53B-F0B8A007A6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{158D722E-2E3D-4BAB-93A7-B487A90FA25B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Predicted Graph" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Experimental Graph" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Controlled variables:</t>
   </si>
@@ -57,9 +58,6 @@
     <t>Determining variability using weight position of 80.1cm:</t>
   </si>
   <si>
-    <t>Force measured by spring scale /N (\pm 0.5N)</t>
-  </si>
-  <si>
     <t>Position of weights along ruler /cm (\pm 0.1cm)</t>
   </si>
   <si>
@@ -67,6 +65,27 @@
   </si>
   <si>
     <t>PREDICTED force measured by spring scale</t>
+  </si>
+  <si>
+    <t>Force measured by spring scale /N (\pm 0.3N)</t>
+  </si>
+  <si>
+    <t>max slope x</t>
+  </si>
+  <si>
+    <t>max slope y</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>min slope x</t>
+  </si>
+  <si>
+    <t>min slope y</t>
   </si>
 </sst>
 </file>
@@ -313,15 +332,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="7.0000000000000007E-2"/>
-            <c:backward val="0.1"/>
+            <c:backward val="0.2"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.10758062479964532"/>
-                  <c:y val="4.2801672141602437E-2"/>
+                  <c:x val="-3.4457011285672245E-2"/>
+                  <c:y val="1.7283791451693641E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -779,7 +797,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
-          <c:min val="0.1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1067,7 +1085,1131 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:backward val="0.2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.1467393624792028E-2"/>
+                  <c:y val="-0.11086899993558899"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="0.30000000000000004"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0000000000000002E-3"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$M$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9B84-4DC4-9653-DCF9B44782E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>max slope line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:backward val="0.2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.9178721796581122E-2"/>
+                  <c:y val="3.5126901615762089E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$3:$O$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0" formatCode="0.000">
+                  <c:v>0.20100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="0.000">
+                  <c:v>0.82899999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="0.0">
+                  <c:v>10.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-03B5-4FE4-B43E-187860DCB511}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>min slope line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:backward val="0.2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.4516782019418217E-2"/>
+                  <c:y val="9.4460573703291084E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$3:$Q$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0" formatCode="0.000">
+                  <c:v>0.19900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="0.000">
+                  <c:v>0.83099999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$3:$R$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="0.0">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-03B5-4FE4-B43E-187860DCB511}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="864030256"/>
+        <c:axId val="796233712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="864030256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Distance between weights and pivot point along ruler /m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="796233712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="796233712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Force measured by spring balance /N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="864030256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1623,8 +2765,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C972303E-BC49-4138-9202-7CB5C9F6842E}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D78D0427-80DA-4288-B67A-77B2AE0E3C5B}">
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0" zoomToFit="1"/>
@@ -1639,13 +3309,46 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8661400" cy="6286500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435BEC99-3BF0-C9B0-F414-6DB2D5B5806F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
     <xdr:ext cx="8665882" cy="6287745"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435BEC99-3BF0-C9B0-F414-6DB2D5B5806F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D3525EF-E8B1-A918-358F-D0747576F593}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1935,10 +3638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView topLeftCell="L30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X37" sqref="X37"/>
+    <sheetView topLeftCell="E34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R67" sqref="R67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1953,15 +3656,21 @@
     <col min="18" max="18" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1975,19 +3684,31 @@
         <v>4</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>10</v>
       </c>
@@ -2014,8 +3735,24 @@
         <f>0.75+(10*(L3-0.1)/0.8)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O3" s="12">
+        <f>L3+0.001</f>
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="P3" s="11">
+        <f>M3-0.3</f>
+        <v>1.7</v>
+      </c>
+      <c r="Q3" s="12">
+        <f>L3-0.001</f>
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="R3" s="11">
+        <f>M3+0.3</f>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E4" s="9">
         <v>9.6999999999999993</v>
       </c>
@@ -2034,7 +3771,7 @@
         <v>2.125</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E5" s="9">
         <v>9.4</v>
       </c>
@@ -2053,7 +3790,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E6" s="10">
         <v>9.1999999999999993</v>
       </c>
@@ -2072,7 +3809,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K7" s="11">
         <v>24</v>
       </c>
@@ -2088,7 +3825,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K8" s="11">
         <v>25</v>
       </c>
@@ -2104,7 +3841,7 @@
         <v>2.625</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K9" s="11">
         <v>26</v>
       </c>
@@ -2120,7 +3857,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K10" s="11">
         <v>27</v>
       </c>
@@ -2136,7 +3873,7 @@
         <v>2.875</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K11" s="11">
         <v>28</v>
       </c>
@@ -2152,7 +3889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K12" s="11">
         <v>29</v>
       </c>
@@ -2168,7 +3905,7 @@
         <v>3.1249999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K13" s="11">
         <v>30</v>
       </c>
@@ -2184,7 +3921,7 @@
         <v>3.2499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K14" s="11">
         <v>31</v>
       </c>
@@ -2200,7 +3937,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K15" s="11">
         <v>32</v>
       </c>
@@ -2216,7 +3953,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K16" s="11">
         <v>33</v>
       </c>
@@ -3000,7 +4737,7 @@
         <v>9.625</v>
       </c>
     </row>
-    <row r="65" spans="11:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="11:18" x14ac:dyDescent="0.35">
       <c r="K65" s="11">
         <v>82</v>
       </c>
@@ -3016,7 +4753,7 @@
         <v>9.7499999999999982</v>
       </c>
     </row>
-    <row r="66" spans="11:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="11:18" x14ac:dyDescent="0.35">
       <c r="K66" s="11">
         <v>83</v>
       </c>
@@ -3030,6 +4767,22 @@
       <c r="N66" s="11">
         <f t="shared" si="1"/>
         <v>9.875</v>
+      </c>
+      <c r="O66" s="12">
+        <f>L66-0.001</f>
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="P66" s="11">
+        <f>M66+0.3</f>
+        <v>10.3</v>
+      </c>
+      <c r="Q66" s="12">
+        <f>L66+0.001</f>
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="R66" s="11">
+        <f>M66-0.3</f>
+        <v>9.6999999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>